<commit_message>
using tag to separate exporting
</commit_message>
<xml_diff>
--- a/TestData/bull_fight_cfg.xlsx
+++ b/TestData/bull_fight_cfg.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -30,123 +30,139 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lucy1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lucy2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能大召3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能大召4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复活时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assets/PG/Common/test.bytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[CONFIG_BEGIN]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[CONFIG_END]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[TABLE_BEGIN]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[TABLE_END]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>索引</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>round(client_only)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rebornTime()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>索引</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>法力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>说明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lucy1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lucy2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能大召3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能大召4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fix64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>round</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>复活时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>资源路径</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>path</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Assets/PG/Common/test.bytes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[CONFIG_BEGIN]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[CONFIG_END]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[TABLE_BEGIN]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[TABLE_END]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RebornTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillDesc</t>
+    <t>测试1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test2(</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>path(cl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp(server_only)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -498,24 +514,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -526,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -534,13 +550,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>4.4000000000000004</v>
@@ -548,286 +564,314 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>8.5</v>
-      </c>
-      <c r="D13">
-        <v>3.3</v>
-      </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>9.5</v>
-      </c>
-      <c r="D14">
-        <v>4.3</v>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>8.5</v>
+      </c>
+      <c r="D15">
+        <v>3.3</v>
+      </c>
+      <c r="E15" t="s">
         <v>9</v>
-      </c>
-      <c r="C15">
-        <v>10.5</v>
-      </c>
-      <c r="D15">
-        <v>5.3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>9.5</v>
+      </c>
+      <c r="D16">
+        <v>4.3</v>
+      </c>
+      <c r="E16" t="s">
         <v>10</v>
-      </c>
-      <c r="C16">
-        <v>11.5</v>
-      </c>
-      <c r="D16">
-        <v>6.3</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>10.5</v>
+      </c>
+      <c r="D17">
+        <v>5.3</v>
+      </c>
+      <c r="E17" t="s">
         <v>9</v>
-      </c>
-      <c r="C17">
-        <v>12.5</v>
-      </c>
-      <c r="D17">
-        <v>7.3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>11.5</v>
+      </c>
+      <c r="D18">
+        <v>6.3</v>
+      </c>
+      <c r="E18" t="s">
         <v>10</v>
-      </c>
-      <c r="C18">
-        <v>13.5</v>
-      </c>
-      <c r="D18">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19">
+        <v>12.5</v>
+      </c>
+      <c r="D19">
+        <v>7.3</v>
+      </c>
+      <c r="E19" t="s">
         <v>9</v>
-      </c>
-      <c r="C19">
-        <v>14.5</v>
-      </c>
-      <c r="D19">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20">
+        <v>13.5</v>
+      </c>
+      <c r="D20">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E20" t="s">
         <v>10</v>
-      </c>
-      <c r="C20">
-        <v>15.5</v>
-      </c>
-      <c r="D20">
-        <v>10.3</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>14.5</v>
+      </c>
+      <c r="D21">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E21" t="s">
         <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21">
-        <v>16.5</v>
-      </c>
-      <c r="D21">
-        <v>11.3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>15.5</v>
+      </c>
+      <c r="D22">
+        <v>10.3</v>
+      </c>
+      <c r="E22" t="s">
         <v>10</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <v>17.5</v>
-      </c>
-      <c r="D22">
-        <v>12.3</v>
-      </c>
-      <c r="E22" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>16.5</v>
+      </c>
+      <c r="D23">
+        <v>11.3</v>
+      </c>
+      <c r="E23" t="s">
         <v>9</v>
-      </c>
-      <c r="C23">
-        <v>18.5</v>
-      </c>
-      <c r="D23">
-        <v>13.3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>17.5</v>
+      </c>
+      <c r="D24">
+        <v>12.3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>18.5</v>
+      </c>
+      <c r="D25">
+        <v>13.3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26">
         <v>12</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>19.5</v>
+      </c>
+      <c r="D26">
+        <v>14.3</v>
+      </c>
+      <c r="E26" t="s">
         <v>10</v>
       </c>
-      <c r="C24">
-        <v>19.5</v>
-      </c>
-      <c r="D24">
-        <v>14.3</v>
-      </c>
-      <c r="E24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>30</v>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>